<commit_message>
Add temporary file for SerialKiller_Dataset.xlsx
</commit_message>
<xml_diff>
--- a/SerialKiller_Dataset.xlsx
+++ b/SerialKiller_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\MAL_FH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02A7EDB3-4970-40E2-8915-CA55E22978FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909BAAC8-0575-4322-8BF0-F05F74A57E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB844A2A-4495-46ED-B84C-4E57A4D07226}"/>
   </bookViews>
@@ -8977,22 +8977,22 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -9370,8 +9370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534861A4-C989-4CC0-97FF-46BA75425A08}">
   <dimension ref="A1:R640"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" workbookViewId="0">
-      <selection activeCell="I623" sqref="I623"/>
+    <sheetView tabSelected="1" topLeftCell="A597" workbookViewId="0">
+      <selection activeCell="I597" sqref="I597"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38527,7 +38527,10 @@
       <c r="H518" s="6">
         <v>1940</v>
       </c>
-      <c r="I518" s="6"/>
+      <c r="I518" s="6">
+        <f>H518-G518</f>
+        <v>43</v>
+      </c>
       <c r="J518" s="6" t="s">
         <v>35</v>
       </c>
@@ -38723,7 +38726,10 @@
       <c r="H522" s="6">
         <v>1995</v>
       </c>
-      <c r="I522" s="6"/>
+      <c r="I522" s="6">
+        <f>H522-G522</f>
+        <v>26</v>
+      </c>
       <c r="J522" s="6" t="s">
         <v>88</v>
       </c>
@@ -38777,7 +38783,10 @@
       <c r="H523" s="10">
         <v>1975</v>
       </c>
-      <c r="I523" s="10"/>
+      <c r="I523" s="6">
+        <f>H523-G523</f>
+        <v>28</v>
+      </c>
       <c r="J523" s="10" t="s">
         <v>105</v>
       </c>
@@ -38877,7 +38886,10 @@
       <c r="H525" s="10">
         <v>1924</v>
       </c>
-      <c r="I525" s="10"/>
+      <c r="I525" s="6">
+        <f>H525-G525</f>
+        <v>34</v>
+      </c>
       <c r="J525" s="10" t="s">
         <v>130</v>
       </c>
@@ -39025,7 +39037,10 @@
       <c r="H528" s="6">
         <v>2009</v>
       </c>
-      <c r="I528" s="6"/>
+      <c r="I528" s="6">
+        <f>H528-G528</f>
+        <v>29</v>
+      </c>
       <c r="J528" s="6" t="s">
         <v>167</v>
       </c>
@@ -39077,7 +39092,10 @@
       <c r="H529" s="10">
         <v>1945</v>
       </c>
-      <c r="I529" s="10"/>
+      <c r="I529" s="6">
+        <f>H529-G529</f>
+        <v>35</v>
+      </c>
       <c r="J529" s="10" t="s">
         <v>189</v>
       </c>
@@ -39131,7 +39149,10 @@
       <c r="H530" s="6">
         <v>1968</v>
       </c>
-      <c r="I530" s="6"/>
+      <c r="I530" s="6">
+        <f>H530-G530</f>
+        <v>43</v>
+      </c>
       <c r="J530" s="6" t="s">
         <v>204</v>
       </c>
@@ -39227,7 +39248,10 @@
       <c r="H532" s="6">
         <v>2005</v>
       </c>
-      <c r="I532" s="6"/>
+      <c r="I532" s="6">
+        <f>H532-G532</f>
+        <v>24</v>
+      </c>
       <c r="J532" s="6" t="s">
         <v>251</v>
       </c>
@@ -39379,7 +39403,10 @@
       <c r="H535" s="10">
         <v>2003</v>
       </c>
-      <c r="I535" s="10"/>
+      <c r="I535" s="6">
+        <f>H535-G535</f>
+        <v>25</v>
+      </c>
       <c r="J535" s="10" t="s">
         <v>274</v>
       </c>
@@ -39477,7 +39504,10 @@
       <c r="H537" s="10">
         <v>1974</v>
       </c>
-      <c r="I537" s="10"/>
+      <c r="I537" s="6">
+        <f>H537-G537</f>
+        <v>22</v>
+      </c>
       <c r="J537" s="10" t="s">
         <v>293</v>
       </c>
@@ -39527,7 +39557,10 @@
       <c r="H538" s="6">
         <v>1962</v>
       </c>
-      <c r="I538" s="6"/>
+      <c r="I538" s="6">
+        <f>H538-G538</f>
+        <v>31</v>
+      </c>
       <c r="J538" s="6" t="s">
         <v>309</v>
       </c>
@@ -39579,7 +39612,10 @@
       <c r="H539" s="10">
         <v>1978</v>
       </c>
-      <c r="I539" s="10"/>
+      <c r="I539" s="6">
+        <f>H539-G539</f>
+        <v>25</v>
+      </c>
       <c r="J539" s="10" t="s">
         <v>320</v>
       </c>
@@ -39629,7 +39665,10 @@
       <c r="H540" s="6">
         <v>2004</v>
       </c>
-      <c r="I540" s="6"/>
+      <c r="I540" s="6">
+        <f>H540-G540</f>
+        <v>48</v>
+      </c>
       <c r="J540" s="6" t="s">
         <v>341</v>
       </c>
@@ -39725,7 +39764,10 @@
       <c r="H542" s="6">
         <v>1990</v>
       </c>
-      <c r="I542" s="6"/>
+      <c r="I542" s="6">
+        <f>H542-G542</f>
+        <v>28</v>
+      </c>
       <c r="J542" s="6" t="s">
         <v>349</v>
       </c>
@@ -39775,7 +39817,10 @@
       <c r="H543" s="10">
         <v>2007</v>
       </c>
-      <c r="I543" s="10"/>
+      <c r="I543" s="6">
+        <f>H543-G543</f>
+        <v>36</v>
+      </c>
       <c r="J543" s="10" t="s">
         <v>352</v>
       </c>
@@ -39871,7 +39916,10 @@
       <c r="H545" s="10">
         <v>1980</v>
       </c>
-      <c r="I545" s="10"/>
+      <c r="I545" s="6">
+        <f>H545-G545</f>
+        <v>36</v>
+      </c>
       <c r="J545" s="10" t="s">
         <v>360</v>
       </c>
@@ -39923,7 +39971,10 @@
       <c r="H546" s="6">
         <v>1991</v>
       </c>
-      <c r="I546" s="6"/>
+      <c r="I546" s="6">
+        <f>H546-G546</f>
+        <v>41</v>
+      </c>
       <c r="J546" s="6" t="s">
         <v>382</v>
       </c>
@@ -39973,7 +40024,10 @@
       <c r="H547" s="10">
         <v>1990</v>
       </c>
-      <c r="I547" s="10"/>
+      <c r="I547" s="6">
+        <f>H547-G547</f>
+        <v>35</v>
+      </c>
       <c r="J547" s="10" t="s">
         <v>411</v>
       </c>
@@ -40021,7 +40075,10 @@
       <c r="H548" s="6">
         <v>1975</v>
       </c>
-      <c r="I548" s="6"/>
+      <c r="I548" s="6">
+        <f>H548-G548</f>
+        <v>21</v>
+      </c>
       <c r="J548" s="6" t="s">
         <v>413</v>
       </c>
@@ -40217,7 +40274,10 @@
       <c r="H552" s="6">
         <v>2008</v>
       </c>
-      <c r="I552" s="6"/>
+      <c r="I552" s="6">
+        <f>H552-G552</f>
+        <v>52</v>
+      </c>
       <c r="J552" s="6" t="s">
         <v>459</v>
       </c>
@@ -40271,7 +40331,10 @@
       <c r="H553" s="10">
         <v>1964</v>
       </c>
-      <c r="I553" s="10"/>
+      <c r="I553" s="6">
+        <f>H553-G553</f>
+        <v>20</v>
+      </c>
       <c r="J553" s="10" t="s">
         <v>470</v>
       </c>
@@ -40367,7 +40430,10 @@
       <c r="H555" s="10">
         <v>1938</v>
       </c>
-      <c r="I555" s="10"/>
+      <c r="I555" s="6">
+        <f>H555-G555</f>
+        <v>14</v>
+      </c>
       <c r="J555" s="10" t="s">
         <v>523</v>
       </c>
@@ -40469,7 +40535,10 @@
       <c r="H557" s="10">
         <v>2008</v>
       </c>
-      <c r="I557" s="10"/>
+      <c r="I557" s="6">
+        <f>H557-G557</f>
+        <v>32</v>
+      </c>
       <c r="J557" s="10" t="s">
         <v>538</v>
       </c>
@@ -40517,7 +40586,10 @@
       <c r="H558" s="6">
         <v>2000</v>
       </c>
-      <c r="I558" s="6"/>
+      <c r="I558" s="6">
+        <f>H558-G558</f>
+        <v>27</v>
+      </c>
       <c r="J558" s="6" t="s">
         <v>552</v>
       </c>
@@ -40617,7 +40689,10 @@
       <c r="H560" s="6">
         <v>1979</v>
       </c>
-      <c r="I560" s="6"/>
+      <c r="I560" s="6">
+        <f>H560-G560</f>
+        <v>34</v>
+      </c>
       <c r="J560" s="6" t="s">
         <v>575</v>
       </c>
@@ -40669,7 +40744,10 @@
       <c r="H561" s="10">
         <v>2004</v>
       </c>
-      <c r="I561" s="10"/>
+      <c r="I561" s="6">
+        <f>H561-G561</f>
+        <v>40</v>
+      </c>
       <c r="J561" s="10" t="s">
         <v>596</v>
       </c>
@@ -40717,7 +40795,10 @@
       <c r="H562" s="6">
         <v>1997</v>
       </c>
-      <c r="I562" s="6"/>
+      <c r="I562" s="6">
+        <f>H562-G562</f>
+        <v>19</v>
+      </c>
       <c r="J562" s="6" t="s">
         <v>612</v>
       </c>
@@ -40811,7 +40892,10 @@
       <c r="H564" s="6">
         <v>1995</v>
       </c>
-      <c r="I564" s="6"/>
+      <c r="I564" s="6">
+        <f>H564-G564</f>
+        <v>22</v>
+      </c>
       <c r="J564" s="6" t="s">
         <v>631</v>
       </c>
@@ -40861,7 +40945,10 @@
       <c r="H565" s="10">
         <v>1986</v>
       </c>
-      <c r="I565" s="10"/>
+      <c r="I565" s="6">
+        <f>H565-G565</f>
+        <v>35</v>
+      </c>
       <c r="J565" s="10" t="s">
         <v>666</v>
       </c>
@@ -41357,7 +41444,10 @@
       <c r="H575" s="10">
         <v>2002</v>
       </c>
-      <c r="I575" s="10"/>
+      <c r="I575" s="6">
+        <f>H575-G575</f>
+        <v>31</v>
+      </c>
       <c r="J575" s="10" t="s">
         <v>831</v>
       </c>
@@ -41411,7 +41501,10 @@
       <c r="H576" s="6">
         <v>2005</v>
       </c>
-      <c r="I576" s="6"/>
+      <c r="I576" s="6">
+        <f t="shared" ref="I576:I582" si="0">H576-G576</f>
+        <v>32</v>
+      </c>
       <c r="J576" s="6" t="s">
         <v>850</v>
       </c>
@@ -41461,7 +41554,10 @@
       <c r="H577" s="10">
         <v>1990</v>
       </c>
-      <c r="I577" s="10"/>
+      <c r="I577" s="6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="J577" s="10" t="s">
         <v>853</v>
       </c>
@@ -41513,7 +41609,10 @@
       <c r="H578" s="6">
         <v>2000</v>
       </c>
-      <c r="I578" s="6"/>
+      <c r="I578" s="6">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
       <c r="J578" s="6" t="s">
         <v>867</v>
       </c>
@@ -41563,7 +41662,10 @@
       <c r="H579" s="10">
         <v>2014</v>
       </c>
-      <c r="I579" s="10"/>
+      <c r="I579" s="6">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
       <c r="J579" s="10" t="s">
         <v>870</v>
       </c>
@@ -41665,7 +41767,10 @@
       <c r="H581" s="10">
         <v>1989</v>
       </c>
-      <c r="I581" s="10"/>
+      <c r="I581" s="6">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
       <c r="J581" s="10" t="s">
         <v>929</v>
       </c>
@@ -41715,7 +41820,10 @@
       <c r="H582" s="6">
         <v>2000</v>
       </c>
-      <c r="I582" s="6"/>
+      <c r="I582" s="6">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
       <c r="J582" s="6" t="s">
         <v>939</v>
       </c>
@@ -41961,7 +42069,10 @@
       <c r="H587" s="10">
         <v>1981</v>
       </c>
-      <c r="I587" s="10"/>
+      <c r="I587" s="6">
+        <f t="shared" ref="I587" si="1">H587-G587</f>
+        <v>28</v>
+      </c>
       <c r="J587" s="10" t="s">
         <v>981</v>
       </c>
@@ -42061,7 +42172,10 @@
       <c r="H589" s="10">
         <v>1917</v>
       </c>
-      <c r="I589" s="10"/>
+      <c r="I589" s="6">
+        <f t="shared" ref="I589" si="2">H589-G589</f>
+        <v>17</v>
+      </c>
       <c r="J589" s="10" t="s">
         <v>1032</v>
       </c>
@@ -42161,7 +42275,10 @@
       <c r="H591" s="10">
         <v>1990</v>
       </c>
-      <c r="I591" s="10"/>
+      <c r="I591" s="6">
+        <f t="shared" ref="I591:I594" si="3">H591-G591</f>
+        <v>25</v>
+      </c>
       <c r="J591" s="10" t="s">
         <v>1044</v>
       </c>
@@ -42213,7 +42330,10 @@
       <c r="H592" s="6">
         <v>1960</v>
       </c>
-      <c r="I592" s="6"/>
+      <c r="I592" s="6">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
       <c r="J592" s="6" t="s">
         <v>1046</v>
       </c>
@@ -42265,7 +42385,10 @@
       <c r="H593" s="10">
         <v>2007</v>
       </c>
-      <c r="I593" s="10"/>
+      <c r="I593" s="6">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
       <c r="J593" s="10" t="s">
         <v>1050</v>
       </c>
@@ -42317,7 +42440,10 @@
       <c r="H594" s="6">
         <v>2005</v>
       </c>
-      <c r="I594" s="6"/>
+      <c r="I594" s="6">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
       <c r="J594" s="6" t="s">
         <v>1054</v>
       </c>
@@ -42469,7 +42595,10 @@
       <c r="H597" s="10">
         <v>1998</v>
       </c>
-      <c r="I597" s="10"/>
+      <c r="I597" s="6">
+        <f t="shared" ref="I597:I600" si="4">H597-G597</f>
+        <v>33</v>
+      </c>
       <c r="J597" s="10" t="s">
         <v>1082</v>
       </c>

</xml_diff>